<commit_message>
20/03/12 add more refs
</commit_message>
<xml_diff>
--- a/FIGs/chapter4/env.xlsx
+++ b/FIGs/chapter4/env.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\x5651\Desktop\2020硕士毕业论文-徐文远\FIGs\chapter4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53F02B2-B62C-4D6C-BAA5-C9AA45FA22F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F33E31C4-1EDD-4DC7-80DA-2700BA169E21}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="12105" activeTab="4" xr2:uid="{8C4E138F-D031-43EA-A9EC-5086CA1E1E9A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="12105" activeTab="2" xr2:uid="{8C4E138F-D031-43EA-A9EC-5086CA1E1E9A}"/>
   </bookViews>
   <sheets>
     <sheet name="env" sheetId="1" r:id="rId1"/>
@@ -280,24 +280,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -320,6 +302,24 @@
     </xf>
     <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -651,16 +651,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
+      <c r="B1" s="13"/>
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="14" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -671,7 +671,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="5"/>
+      <c r="A3" s="14"/>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
@@ -680,7 +680,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
+      <c r="A4" s="15"/>
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
@@ -689,7 +689,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="14" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -700,7 +700,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
+      <c r="A6" s="14"/>
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
@@ -709,7 +709,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
+      <c r="A7" s="15"/>
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
@@ -739,46 +739,46 @@
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="7"/>
-      <c r="B1" s="7"/>
-      <c r="C1" s="8" t="s">
+      <c r="A1" s="16"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="8"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="10" t="s">
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
-      <c r="B4" s="10" t="s">
+      <c r="A4" s="15"/>
+      <c r="B4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -797,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F46561C-F877-4B81-A23C-562E66ED39C0}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G4" sqref="A1:G4"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -814,22 +814,22 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="3"/>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="8" t="s">
         <v>29</v>
       </c>
     </row>
@@ -837,47 +837,47 @@
       <c r="A2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="6">
         <v>10769</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="6">
         <v>6377</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="6">
         <f>B2-C2</f>
         <v>4392</v>
       </c>
-      <c r="E2" s="12">
+      <c r="E2" s="6">
         <v>3501</v>
       </c>
-      <c r="F2" s="12">
+      <c r="F2" s="6">
         <v>6377</v>
       </c>
-      <c r="G2" s="12">
-        <f>SUM(F2:F2)</f>
-        <v>6377</v>
+      <c r="G2" s="6">
+        <f>SUM(E2:F2)</f>
+        <v>9878</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="6">
         <v>5217</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="6">
         <v>550</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="6">
         <v>3823</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="6">
         <f>SUM(E3:F3)</f>
         <v>4373</v>
       </c>
@@ -886,24 +886,24 @@
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="7">
         <f>SUM(E2:E3)</f>
         <v>4051</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="7">
         <f>F2+E3</f>
         <v>6927</v>
       </c>
-      <c r="G4" s="13">
+      <c r="G4" s="7">
         <f>SUM(E4:F4)</f>
         <v>10978</v>
       </c>
@@ -947,16 +947,16 @@
       <c r="A2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="9">
         <v>0.68400000000000005</v>
       </c>
-      <c r="C2" s="15">
+      <c r="C2" s="9">
         <v>0.65090000000000003</v>
       </c>
-      <c r="D2" s="18">
+      <c r="D2" s="12">
         <v>1</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="9">
         <v>0.78510000000000002</v>
       </c>
       <c r="I2">
@@ -976,16 +976,16 @@
       <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="17">
+      <c r="B3" s="11">
         <v>0.87839999999999996</v>
       </c>
-      <c r="C3" s="17">
+      <c r="C3" s="11">
         <v>0.90529999999999999</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="10">
         <v>0.88649999999999995</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="11">
         <v>0.89580000000000004</v>
       </c>
       <c r="I3">
@@ -1103,8 +1103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0D23D5E-1337-43F2-8C80-CA8A1BFCE674}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1118,14 +1118,14 @@
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="19"/>
       <c r="B1" s="19"/>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="4"/>
+      <c r="D1" s="13"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
       <c r="C2" s="1" t="s">
         <v>28</v>
       </c>
@@ -1134,7 +1134,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="14" t="s">
         <v>37</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1147,10 +1147,10 @@
         <v>92</v>
       </c>
       <c r="F3">
-        <v>629</v>
+        <v>661</v>
       </c>
       <c r="G3">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="H3">
         <v>80</v>
@@ -1160,7 +1160,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
+      <c r="A4" s="15"/>
       <c r="B4" s="1" t="s">
         <v>36</v>
       </c>
@@ -1171,48 +1171,48 @@
         <v>655</v>
       </c>
       <c r="F4">
-        <v>673</v>
+        <v>653</v>
       </c>
       <c r="G4">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="H4">
-        <v>111</v>
+        <v>76</v>
       </c>
       <c r="I4">
-        <v>85</v>
+        <v>334</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F5">
-        <v>664</v>
+        <v>650</v>
       </c>
       <c r="G5">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="H5">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="I5">
-        <v>324</v>
+        <v>333</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F6">
         <f>AVERAGE(F3:F5)</f>
-        <v>655.33333333333337</v>
+        <v>654.66666666666663</v>
       </c>
       <c r="G6">
         <f t="shared" ref="G6:I6" si="0">AVERAGE(G3:G5)</f>
-        <v>31.666666666666668</v>
+        <v>35</v>
       </c>
       <c r="H6">
         <f t="shared" si="0"/>
-        <v>92.333333333333329</v>
+        <v>79.333333333333329</v>
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>243</v>
+        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -1223,5 +1223,6 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>